<commit_message>
Add funções de térmica.
</commit_message>
<xml_diff>
--- a/dados_tabelas/excent_adm.xlsx
+++ b/dados_tabelas/excent_adm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaque\Desktop\Elementos_II\mancais\dados_tabelas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B0DB8A-D7F1-4EFC-9578-047F17EE94EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3420EF4C-D003-4C65-BEAD-110240FCE43D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2013683D-42BF-4558-BA95-970AAD469545}"/>
   </bookViews>
@@ -404,13 +404,14 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
   </cols>
@@ -434,19 +435,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0</v>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>